<commit_message>
AT: % LU by missing/nonmissing net returns values, kernel density graphs
</commit_message>
<xml_diff>
--- a/results/initial_descriptives/combined/dataObsStats.xlsx
+++ b/results/initial_descriptives/combined/dataObsStats.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\GitRepos\land-use\results\initial_descriptives\combined\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E48CCC4C-8FD7-4E8B-9DB4-C05A33D0B501}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1260AF1D-445A-4DD9-93EC-0106AB787FFB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="county-year" sheetId="1" r:id="rId1"/>

</xml_diff>

<commit_message>
incorporate new urban returns, use 2000 data for 2002
</commit_message>
<xml_diff>
--- a/results/initial_descriptives/combined/dataObsStats.xlsx
+++ b/results/initial_descriptives/combined/dataObsStats.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="414" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="552" uniqueCount="43">
   <si>
     <t>year</t>
   </si>
@@ -6845,10 +6845,10 @@
         <v>2002</v>
       </c>
       <c r="B6" s="1">
-        <v>0</v>
+        <v>2069</v>
       </c>
       <c r="C6" s="1">
-        <v>0</v>
+        <v>67.350257873535156</v>
       </c>
       <c r="D6" s="1">
         <v>3072</v>
@@ -6896,16 +6896,16 @@
         <v>16.536458969116211</v>
       </c>
       <c r="S6" s="1">
-        <v>0</v>
+        <v>3072</v>
       </c>
       <c r="T6" s="1">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="U6" s="1">
-        <v>3072</v>
+        <v>0</v>
       </c>
       <c r="V6" s="1">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="W6" s="1">
         <v>3065</v>
@@ -7342,10 +7342,10 @@
     </row>
     <row r="2">
       <c r="A2" s="1">
-        <v>4054</v>
+        <v>6123</v>
       </c>
       <c r="B2" s="1">
-        <v>16.495767593383789</v>
+        <v>24.91455078125</v>
       </c>
       <c r="C2" s="1">
         <v>24576</v>
@@ -7393,16 +7393,16 @@
         <v>68.701171875</v>
       </c>
       <c r="R2" s="1">
-        <v>9155</v>
+        <v>12227</v>
       </c>
       <c r="S2" s="1">
-        <v>37.251789093017578</v>
+        <v>49.751789093017578</v>
       </c>
       <c r="T2" s="1">
-        <v>15421</v>
+        <v>12349</v>
       </c>
       <c r="U2" s="1">
-        <v>62.748210906982422</v>
+        <v>50.248210906982422</v>
       </c>
       <c r="V2" s="1">
         <v>21455</v>
@@ -7938,10 +7938,10 @@
         <v>2002</v>
       </c>
       <c r="B6" s="1">
-        <v>0</v>
+        <v>929707</v>
       </c>
       <c r="C6" s="1">
-        <v>0</v>
+        <v>68.2293701171875</v>
       </c>
       <c r="D6" s="1">
         <v>1362620</v>
@@ -7989,16 +7989,16 @@
         <v>17.834098815917969</v>
       </c>
       <c r="S6" s="1">
-        <v>0</v>
+        <v>1362620</v>
       </c>
       <c r="T6" s="1">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="U6" s="1">
-        <v>1362620</v>
+        <v>0</v>
       </c>
       <c r="V6" s="1">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="W6" s="1">
         <v>1361164</v>
@@ -8435,10 +8435,10 @@
     </row>
     <row r="2">
       <c r="A2" s="1">
-        <v>1820234</v>
+        <v>2749941</v>
       </c>
       <c r="B2" s="1">
-        <v>16.69792366027832</v>
+        <v>25.226594924926758</v>
       </c>
       <c r="C2" s="1">
         <v>10900960</v>
@@ -8486,16 +8486,16 @@
         <v>69.187789916992188</v>
       </c>
       <c r="R2" s="1">
-        <v>4054753</v>
+        <v>5417373</v>
       </c>
       <c r="S2" s="1">
-        <v>37.196292877197266</v>
+        <v>49.696292877197266</v>
       </c>
       <c r="T2" s="1">
-        <v>6846207</v>
+        <v>5483587</v>
       </c>
       <c r="U2" s="1">
-        <v>62.803707122802734</v>
+        <v>50.303707122802734</v>
       </c>
       <c r="V2" s="1">
         <v>9528148</v>

</xml_diff>